<commit_message>
E4 - Device Update
</commit_message>
<xml_diff>
--- a/E4/E4.Device/PDO Mappings.xlsx
+++ b/E4/E4.Device/PDO Mappings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="13980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="13980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Laser Robot" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="73">
   <si>
     <t>RPDOs</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Row / Col; 0x2410, 0x01</t>
   </si>
   <si>
-    <t>BLDC 0/1 Control / Target Torque</t>
-  </si>
-  <si>
     <t>IMU Data + MCU Temp</t>
   </si>
   <si>
@@ -156,15 +153,9 @@
     <t>IMU Yaw Val; 0x2441, 0x03 (int16_t)</t>
   </si>
   <si>
-    <t>BLDC 0 Control Word; 0x6040; (uint16_t)</t>
-  </si>
-  <si>
     <t>BLDC 0 Target Torque; 0x6071 (uint16_t)</t>
   </si>
   <si>
-    <t>BLDC 1 Control Word; 0x6840; (uint16_t)</t>
-  </si>
-  <si>
     <t>BLDC 1 Target Torque; 0x6871 (uint16_t)</t>
   </si>
   <si>
@@ -231,16 +222,28 @@
     <t>Laser Scanner Status + Readings</t>
   </si>
   <si>
-    <t>IMU Yaw Val; 0x2445, 0x03 (int16_t)</t>
-  </si>
-  <si>
-    <t>IMU Pitch Val; 0x2445, 0x02 (int16_t)</t>
-  </si>
-  <si>
     <t>Main Board IMU Data + MCU Temp</t>
   </si>
   <si>
     <t>Target IMU Data + Laser Position</t>
+  </si>
+  <si>
+    <t>Target IMU Pitch Val; 0x2445, 0x02 (int16_t)</t>
+  </si>
+  <si>
+    <t>Target IMU Yaw Val; 0x2445, 0x03 (int16_t)</t>
+  </si>
+  <si>
+    <t>Main IMU Roll Val; 0x2441, 0x01 (int16_t)</t>
+  </si>
+  <si>
+    <t>Main IMU Pitch Val; 0x2441, 0x02 (int16_t)</t>
+  </si>
+  <si>
+    <t>Main IMU Yaw Val; 0x2441, 0x03 (int16_t)</t>
+  </si>
+  <si>
+    <t>BLDC  0/1 Target Torque</t>
   </si>
 </sst>
 </file>
@@ -471,17 +474,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -489,10 +483,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -811,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="C3:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,16 +826,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -876,24 +879,20 @@
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="20"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="13" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,18 +902,18 @@
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="27"/>
+      <c r="C4" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="8" t="s">
         <v>31</v>
       </c>
@@ -926,18 +925,18 @@
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="20"/>
+      <c r="C5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="23"/>
       <c r="K5" s="12" t="s">
         <v>32</v>
       </c>
@@ -1091,22 +1090,22 @@
       <c r="B14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14" s="27"/>
+      <c r="J14" s="25"/>
       <c r="K14" s="8" t="s">
         <v>30</v>
       </c>
@@ -1118,18 +1117,18 @@
       <c r="B15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="20"/>
+      <c r="C15" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="12" t="s">
         <v>27</v>
       </c>
@@ -1141,18 +1140,18 @@
       <c r="B16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="20"/>
+      <c r="C16" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="12" t="s">
         <v>28</v>
       </c>
@@ -1171,7 +1170,7 @@
         <v>22</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1201,24 +1200,24 @@
       <c r="B19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24" t="s">
+      <c r="F19" s="21"/>
+      <c r="G19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="24"/>
+      <c r="H19" s="21"/>
       <c r="I19" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1228,20 +1227,20 @@
       <c r="B20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="21"/>
+      <c r="C20" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="24"/>
       <c r="G20" s="4"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
       <c r="J20" s="11"/>
       <c r="K20" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1251,20 +1250,20 @@
       <c r="B21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="21"/>
+      <c r="C21" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="24"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
       <c r="J21" s="19"/>
       <c r="K21" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1286,6 +1285,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="G16:J16"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="C3:D3"/>
@@ -1299,17 +1309,6 @@
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1320,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,16 +1331,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1385,24 +1384,20 @@
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="20"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="13" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1412,18 +1407,18 @@
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="27"/>
+      <c r="C4" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="8" t="s">
         <v>31</v>
       </c>
@@ -1435,18 +1430,18 @@
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="20"/>
+      <c r="C5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="23"/>
       <c r="K5" s="12" t="s">
         <v>32</v>
       </c>
@@ -1600,22 +1595,22 @@
       <c r="B14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14" s="27"/>
+      <c r="J14" s="25"/>
       <c r="K14" s="8" t="s">
         <v>30</v>
       </c>
@@ -1627,18 +1622,18 @@
       <c r="B15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="20"/>
+      <c r="C15" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="12" t="s">
         <v>27</v>
       </c>
@@ -1650,18 +1645,18 @@
       <c r="B16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="20"/>
+      <c r="C16" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="12" t="s">
         <v>28</v>
       </c>
@@ -1680,7 +1675,7 @@
         <v>22</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1710,24 +1705,24 @@
       <c r="B19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="24"/>
+      <c r="C19" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="21"/>
       <c r="I19" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1737,24 +1732,24 @@
       <c r="B20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24" t="s">
+      <c r="C20" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="H20" s="24"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="11" t="s">
         <v>37</v>
       </c>
       <c r="J20" s="11"/>
       <c r="K20" s="16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1764,19 +1759,17 @@
       <c r="B21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="21"/>
+      <c r="C21" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
       <c r="J21" s="19"/>
       <c r="K21" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1798,11 +1791,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="G15:J15"/>
     <mergeCell ref="C16:F16"/>
@@ -1810,19 +1811,11 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G20:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>